<commit_message>
El excel que se me habia pasado xd
</commit_message>
<xml_diff>
--- a/Requisitos-Tareas.xlsx
+++ b/Requisitos-Tareas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="106">
   <si>
     <t xml:space="preserve">ID REQUISITO</t>
   </si>
@@ -366,6 +366,18 @@
   </si>
   <si>
     <t xml:space="preserve">Joaquín</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requisito: Mapa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ver mapa en aplicación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Añadir ubicaciones en el mapa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joaquín/Serena</t>
   </si>
 </sst>
 </file>
@@ -532,7 +544,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -605,6 +617,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -661,23 +677,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -772,11 +796,11 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.14"/>
   </cols>
@@ -1109,7 +1133,7 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1168,8 +1192,8 @@
         <v>71</v>
       </c>
       <c r="M2" s="13" t="n">
-        <f aca="false">SUM(H2,H12,H8,H20,H23)</f>
-        <v>49.5</v>
+        <f aca="false">SUM(H2,H12,H8,H20,H23,H25)</f>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1188,6 +1212,7 @@
       <c r="F3" s="17" t="s">
         <v>74</v>
       </c>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
@@ -1219,7 +1244,7 @@
       <c r="D5" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="19" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1236,36 +1261,36 @@
       <c r="D6" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="19" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="20" t="n">
+      <c r="C7" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="21" t="n">
+      <c r="D7" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="0" t="s">
         <v>69</v>
       </c>
@@ -1282,65 +1307,65 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="20" t="n">
+      <c r="C9" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="21" t="n">
+      <c r="D9" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="20" t="n">
+      <c r="C10" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="21" t="n">
+      <c r="D10" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="20" t="n">
+      <c r="C11" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="21" t="n">
+      <c r="D11" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="0" t="s">
         <v>69</v>
       </c>
@@ -1357,131 +1382,131 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="25" t="n">
+      <c r="C13" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="26" t="n">
+      <c r="D13" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="25" t="n">
+      <c r="C14" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="26" t="n">
+      <c r="D14" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="25" t="n">
+      <c r="C15" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="D15" s="26" t="n">
+      <c r="D15" s="27" t="n">
         <v>1.5</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="25" t="n">
+      <c r="C16" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="26" t="n">
+      <c r="D16" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="25" t="n">
+      <c r="C17" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="D17" s="26" t="n">
+      <c r="D17" s="27" t="n">
         <v>0.5</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="18" t="s">
+      <c r="E17" s="28"/>
+      <c r="F17" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="20" t="n">
+      <c r="C18" s="21" t="n">
         <v>1.5</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="F18" s="22" t="s">
+      <c r="D18" s="22"/>
+      <c r="F18" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="20" t="n">
+      <c r="C19" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="22" t="s">
+      <c r="D19" s="22"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="0" t="s">
         <v>69</v>
       </c>
@@ -1498,22 +1523,22 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="29" t="n">
+      <c r="C21" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="30" t="n">
+      <c r="D21" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="J21" s="32"/>
+      <c r="J21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
@@ -1528,19 +1553,19 @@
       <c r="D22" s="16" t="n">
         <v>8.5</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
       <c r="G23" s="0" t="s">
         <v>69</v>
       </c>
@@ -1550,198 +1575,246 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="25" t="n">
+      <c r="C24" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D24" s="26" t="n">
+      <c r="D24" s="27" t="n">
         <v>3.5</v>
       </c>
       <c r="F24" s="33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">SUM(D26:D27)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <f aca="false">SUM(C26:C27)</f>
+        <v>3</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
+      <c r="A26" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="37" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="37"/>
+      <c r="A27" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="37"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
     </row>
     <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="37"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="40"/>
     </row>
     <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="34"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="40"/>
     </row>
     <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="34"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="37"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="40"/>
     </row>
     <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C34" s="38"/>
-      <c r="D34" s="37"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="40"/>
     </row>
     <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C35" s="38"/>
-      <c r="D35" s="37"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="40"/>
     </row>
     <row r="36" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C36" s="38"/>
-      <c r="D36" s="37"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="40"/>
     </row>
     <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C37" s="38"/>
-      <c r="D37" s="37"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="40"/>
     </row>
     <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C38" s="38"/>
-      <c r="D38" s="37"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="40"/>
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C39" s="38"/>
-      <c r="D39" s="37"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="40"/>
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C40" s="38"/>
-      <c r="D40" s="37"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="40"/>
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="38"/>
-      <c r="D41" s="37"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="40"/>
     </row>
     <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C42" s="38"/>
-      <c r="D42" s="37"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="40"/>
     </row>
     <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="38"/>
-      <c r="D43" s="37"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="40"/>
     </row>
     <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C44" s="38"/>
-      <c r="D44" s="37"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="40"/>
     </row>
     <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="38"/>
-      <c r="D45" s="37"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="40"/>
     </row>
     <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="38"/>
-      <c r="D46" s="37"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="40"/>
     </row>
     <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C47" s="38"/>
-      <c r="D47" s="37"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="40"/>
     </row>
     <row r="48" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="38"/>
-      <c r="D48" s="37"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="40"/>
     </row>
     <row r="49" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C49" s="38"/>
-      <c r="D49" s="37"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="40"/>
     </row>
     <row r="50" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C50" s="38"/>
-      <c r="D50" s="37"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="40"/>
     </row>
     <row r="51" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="38"/>
-      <c r="D51" s="37"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="40"/>
     </row>
     <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="38"/>
-      <c r="D52" s="37"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="40"/>
     </row>
     <row r="53" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="38"/>
-      <c r="D53" s="37"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="40"/>
     </row>
     <row r="54" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="38"/>
-      <c r="D54" s="37"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="40"/>
     </row>
     <row r="55" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="38"/>
-      <c r="D55" s="37"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="40"/>
     </row>
     <row r="56" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="38"/>
-      <c r="D56" s="37"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="40"/>
     </row>
     <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="38"/>
-      <c r="D57" s="37"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="40"/>
     </row>
     <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="38"/>
-      <c r="D58" s="37"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="40"/>
     </row>
     <row r="59" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="38"/>
-      <c r="D59" s="37"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="40"/>
     </row>
     <row r="60" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="38"/>
-      <c r="D60" s="37"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="40"/>
     </row>
     <row r="61" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="38"/>
-      <c r="D61" s="37"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="40"/>
     </row>
     <row r="62" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="38"/>
-      <c r="D62" s="37"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="40"/>
     </row>
     <row r="63" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="38"/>
-      <c r="D63" s="37"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="40"/>
     </row>
     <row r="64" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="38"/>
-      <c r="D64" s="37"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="40"/>
     </row>
     <row r="65" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="38"/>
-      <c r="D65" s="37"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A25:F25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>